<commit_message>
Atualização planilha de reuniões
</commit_message>
<xml_diff>
--- a/projeto/Documentos/Planejamento.xlsx
+++ b/projeto/Documentos/Planejamento.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rhian\Desktop\projeto\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\Nova pasta\Grupo-02-CCO-Luminous--Recome-o\projeto\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3153FB26-0DCB-426E-9924-8848D3F79697}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82367BD-A945-4F75-B571-0AED0DFBA41E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="20460" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planejamento" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="87">
   <si>
     <t>Entregáveis Sprint 1</t>
   </si>
@@ -187,56 +187,116 @@
     <t>1º</t>
   </si>
   <si>
-    <t>Planejar Cronograma</t>
-  </si>
-  <si>
     <t>Ninguem</t>
   </si>
   <si>
     <t>Concluido</t>
   </si>
   <si>
-    <t>Decidiu Metas(09/04)</t>
-  </si>
-  <si>
     <t>18h</t>
   </si>
   <si>
     <t>2º</t>
   </si>
   <si>
-    <t>Atividade Pi</t>
-  </si>
-  <si>
     <t>Feito</t>
   </si>
   <si>
     <t>Primeira Entrega</t>
   </si>
   <si>
-    <t>12h</t>
-  </si>
-  <si>
     <t>Padronização site</t>
   </si>
   <si>
     <t>3º</t>
   </si>
   <si>
-    <t>HLD e LLD e organizar git hub</t>
-  </si>
-  <si>
-    <t>Luiza(Justificada)</t>
-  </si>
-  <si>
     <t>Definição do HLD</t>
+  </si>
+  <si>
+    <t>4º</t>
+  </si>
+  <si>
+    <t>6º</t>
+  </si>
+  <si>
+    <t>Troca de Funções</t>
+  </si>
+  <si>
+    <t>HLD, LLD, organizar git hub, troca de funções.</t>
+  </si>
+  <si>
+    <t>Atividade Pi.</t>
+  </si>
+  <si>
+    <t>Planejar Cronograma.</t>
+  </si>
+  <si>
+    <t>Luiza(Justificada), Willian</t>
+  </si>
+  <si>
+    <t>Decidir Metas(09/04)</t>
+  </si>
+  <si>
+    <t>R.A</t>
+  </si>
+  <si>
+    <t>02 201 002</t>
+  </si>
+  <si>
+    <t>02 201 010</t>
+  </si>
+  <si>
+    <t>02 201 031</t>
+  </si>
+  <si>
+    <t>02 201 041</t>
+  </si>
+  <si>
+    <t>02 201 025</t>
+  </si>
+  <si>
+    <t>02 201 026</t>
+  </si>
+  <si>
+    <t>Integrantes</t>
+  </si>
+  <si>
+    <t>André Moura</t>
+  </si>
+  <si>
+    <t>César Almeida</t>
+  </si>
+  <si>
+    <t>Luiza Vitória</t>
+  </si>
+  <si>
+    <t>Rhian Bottura</t>
+  </si>
+  <si>
+    <t>Vinicius de Carvalho</t>
+  </si>
+  <si>
+    <t>Willian Leal</t>
+  </si>
+  <si>
+    <t>Ninguém</t>
+  </si>
+  <si>
+    <t>Concluído</t>
+  </si>
+  <si>
+    <t>Avanço da planilha dos entregáveis</t>
+  </si>
+  <si>
+    <t>Avançar planilha de entregáveis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,16 +317,19 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -274,8 +337,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,6 +410,30 @@
       <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FFC9DAF8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor rgb="FFC9DAF8"/>
       </patternFill>
     </fill>
   </fills>
@@ -394,10 +500,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -427,14 +534,37 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{496684B7-6141-48EE-B31C-D48032DED8E2}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -880,7 +1010,7 @@
       </c>
       <c r="J12" s="26"/>
       <c r="K12" s="26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
@@ -1015,7 +1145,7 @@
         <v>43923</v>
       </c>
       <c r="M17" s="27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1148,139 +1278,298 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D12C33-BB80-4604-A192-D7E5375EC1AE}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>50</v>
+      <c r="A1" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B10" s="33">
         <v>43922</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C10" s="34">
         <v>0.71527777777777779</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D10" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="F10" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="G10" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="30">
+        <v>1</v>
+      </c>
+      <c r="I10" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="29" t="s">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="29">
+      <c r="B11" s="33">
+        <v>43923</v>
+      </c>
+      <c r="C11" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="30">
         <v>1</v>
       </c>
-      <c r="I2" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="30">
-        <v>43923</v>
-      </c>
-      <c r="C3" s="31" t="s">
+      <c r="I11" s="34">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="33">
+        <v>43926</v>
+      </c>
+      <c r="C12" s="34">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="30">
+        <v>1</v>
+      </c>
+      <c r="I12" s="34">
+        <v>0.89583333333333337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" s="29" t="s">
+      <c r="B13" s="33">
+        <v>43929</v>
+      </c>
+      <c r="C13" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="30"/>
+      <c r="I13" s="34">
+        <v>0.52777777777777779</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="29">
-        <v>1</v>
-      </c>
-      <c r="I3" s="31">
-        <v>0.55208333333333337</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="B14" s="33">
+        <v>43933</v>
+      </c>
+      <c r="C14" s="34">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D14" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="30">
-        <v>43926</v>
-      </c>
-      <c r="C4" s="31">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="29">
-        <v>1</v>
-      </c>
-      <c r="I4" s="31">
-        <v>0.89583333333333337</v>
-      </c>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="36"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="36"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
+  <conditionalFormatting sqref="A1:B1">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{68D009F7-CE16-4D3D-9614-C463BC1881EA}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{68D009F7-CE16-4D3D-9614-C463BC1881EA}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>A1:B1</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>